<commit_message>
Thursday Update: Redo-graphs and feedback from meeting
</commit_message>
<xml_diff>
--- a/data/Tier_2_emission.xlsx
+++ b/data/Tier_2_emission.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chery\Documents\Ariel_Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C25F8E3-6F50-4111-9FC0-B77973572472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB614C2-9E43-449A-A866-7B0D4C505E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5CB49004-E1CD-4DAA-B60B-64ECBA95970C}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t>Tier2_SNR</t>
   </si>
   <si>
-    <t>Tier2 Transit S/N</t>
-  </si>
-  <si>
     <t>HIP 65 A b</t>
   </si>
   <si>
@@ -210,12 +207,18 @@
   </si>
   <si>
     <t>\\</t>
+  </si>
+  <si>
+    <t>Planet Temperature [K]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -262,10 +265,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -583,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41DF0B9-C651-45E3-9934-BB4818A16BF9}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="J52" sqref="A2:J52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -600,1642 +605,1642 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2">
         <v>2.0299999999999998</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2">
         <v>0.9809734</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G2">
+        <v>1361.7577220000001</v>
+      </c>
+      <c r="H2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" s="3">
         <v>49.014415840195603</v>
       </c>
-      <c r="H2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2">
-        <v>7.1918079467876703</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3">
         <v>1.891</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3">
         <v>1.4811235</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G3">
+        <v>3916.2360760000001</v>
+      </c>
+      <c r="H3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" s="3">
         <v>34.596572133369598</v>
       </c>
-      <c r="H3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I3">
-        <v>5.0768228502505304</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4">
         <v>1.593</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4">
         <v>1.21987</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G4">
+        <v>2599.5973770000001</v>
+      </c>
+      <c r="H4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="3">
         <v>31.679892507428701</v>
       </c>
-      <c r="H4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I4">
-        <v>4.4574339776630003</v>
-      </c>
       <c r="J4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5">
         <v>1.619</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5">
         <v>2.7240329999999999</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G5">
+        <v>2606.6433750000001</v>
+      </c>
+      <c r="H5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="3">
         <v>30.308478991610901</v>
       </c>
-      <c r="H5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I5">
-        <v>4.9993476943191899</v>
-      </c>
       <c r="J5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6">
         <v>1.1299999999999999</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6">
         <v>2.2185756699999999</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G6">
+        <v>1162.930605</v>
+      </c>
+      <c r="H6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="3">
         <v>28.586653870594201</v>
       </c>
-      <c r="H6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6">
-        <v>9.6985778540213108</v>
-      </c>
       <c r="J6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7">
         <v>1.7410000000000001</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7">
         <v>3.4741084999999998</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G7">
+        <v>2181.3966270000001</v>
+      </c>
+      <c r="H7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="3">
         <v>22.058675786419801</v>
       </c>
-      <c r="H7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I7">
-        <v>3.1413049319211002</v>
-      </c>
       <c r="J7" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8">
         <v>1.39</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E8">
         <v>3.5247485900000002</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8">
+        <v>1405.9102700000001</v>
+      </c>
+      <c r="H8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="3">
         <v>21.355829696433801</v>
       </c>
-      <c r="H8" t="s">
-        <v>56</v>
-      </c>
-      <c r="I8">
-        <v>14.1300414756212</v>
-      </c>
       <c r="J8" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9">
         <v>1.83</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9">
         <v>1.8098860000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G9">
+        <v>2110.9742860000001</v>
+      </c>
+      <c r="H9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="3">
         <v>18.482245775245001</v>
       </c>
-      <c r="H9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9">
-        <v>6.8940908471756996</v>
-      </c>
       <c r="J9" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10">
         <v>1.24</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10">
         <v>0.94145223</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G10">
+        <v>2408.7462070000001</v>
+      </c>
+      <c r="H10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="3">
         <v>17.852497228859001</v>
       </c>
-      <c r="H10" t="s">
-        <v>56</v>
-      </c>
-      <c r="I10">
-        <v>0.36081381901008402</v>
-      </c>
       <c r="J10" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11">
         <v>1.5</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11">
         <v>2.1487799999999999</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G11">
+        <v>2583.1938180000002</v>
+      </c>
+      <c r="H11" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="3">
         <v>15.9986205162788</v>
       </c>
-      <c r="H11" t="s">
-        <v>56</v>
-      </c>
-      <c r="I11">
-        <v>1.23344322549375</v>
-      </c>
       <c r="J11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12">
         <v>1.7529999999999999</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12">
         <v>1.2749250400000001</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G12">
+        <v>2391.043885</v>
+      </c>
+      <c r="H12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="3">
         <v>15.9416336023656</v>
       </c>
-      <c r="H12" t="s">
-        <v>56</v>
-      </c>
-      <c r="I12">
-        <v>4.3421499646039496</v>
-      </c>
       <c r="J12" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13">
         <v>1.6</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13">
         <v>2.7347700000000001</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G13">
+        <v>1975.1330109999999</v>
+      </c>
+      <c r="H13" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="3">
         <v>15.0477188273692</v>
       </c>
-      <c r="H13" t="s">
-        <v>56</v>
-      </c>
-      <c r="I13">
-        <v>3.9323256158737099</v>
-      </c>
       <c r="J13" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14">
         <v>1.53</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14">
         <v>2.8240599999999998</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G14">
+        <v>2321.685164</v>
+      </c>
+      <c r="H14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" s="3">
         <v>14.8954236981106</v>
       </c>
-      <c r="H14" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14">
-        <v>1.6420779286729501</v>
-      </c>
       <c r="J14" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15">
         <v>1.875</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E15">
         <v>1.902603</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G15">
+        <v>2488.5002690000001</v>
+      </c>
+      <c r="H15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" s="3">
         <v>14.794049921266399</v>
       </c>
-      <c r="H15" t="s">
-        <v>56</v>
-      </c>
-      <c r="I15">
-        <v>2.28555679510163</v>
-      </c>
       <c r="J15" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16">
         <v>2.0699999999999998</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E16">
         <v>3.7650006999999999</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G16">
+        <v>1875.839925</v>
+      </c>
+      <c r="H16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="3">
         <v>13.6994268884118</v>
       </c>
-      <c r="H16" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16">
-        <v>1.5525321449670599</v>
-      </c>
       <c r="J16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17">
         <v>1.23</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E17">
         <v>1.3600285400000001</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G17">
+        <v>1640.5562219999999</v>
+      </c>
+      <c r="H17" t="s">
+        <v>55</v>
+      </c>
+      <c r="I17" s="3">
         <v>13.2185049563824</v>
       </c>
-      <c r="H17" t="s">
-        <v>56</v>
-      </c>
-      <c r="I17">
-        <v>2.23694969920715</v>
-      </c>
       <c r="J17" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18">
         <v>1.9370000000000001</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E18">
         <v>1.0914200000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G18">
+        <v>2499.2724840000001</v>
+      </c>
+      <c r="H18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18" s="3">
         <v>12.557296169805801</v>
       </c>
-      <c r="H18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I18">
-        <v>2.6069363403529699</v>
-      </c>
       <c r="J18" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19">
         <v>1.5449999999999999</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E19">
         <v>3.3089580000000001</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G19">
+        <v>2062.6546939999998</v>
+      </c>
+      <c r="H19" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="3">
         <v>12.451409813379801</v>
       </c>
-      <c r="H19" t="s">
-        <v>56</v>
-      </c>
-      <c r="I19">
-        <v>3.6704120823901301</v>
-      </c>
       <c r="J19" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20">
         <v>1.98</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E20">
         <v>2.1500081999999998</v>
       </c>
       <c r="F20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G20">
+        <v>1777.378359</v>
+      </c>
+      <c r="H20" t="s">
+        <v>55</v>
+      </c>
+      <c r="I20" s="3">
         <v>12.3145282849542</v>
       </c>
-      <c r="H20" t="s">
-        <v>56</v>
-      </c>
-      <c r="I20">
-        <v>8.0092932586559602</v>
-      </c>
       <c r="J20" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21">
         <v>1.49</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E21">
         <v>2.6502370000000002</v>
       </c>
       <c r="F21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G21">
+        <v>2306.1039169999999</v>
+      </c>
+      <c r="H21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" s="3">
         <v>12.2334399254114</v>
       </c>
-      <c r="H21" t="s">
-        <v>56</v>
-      </c>
-      <c r="I21">
-        <v>1.2915805801581599</v>
-      </c>
       <c r="J21" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22">
         <v>1.87</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22">
         <v>2.7443245200000002</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G22">
+        <v>2467.4412189999998</v>
+      </c>
+      <c r="H22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I22" s="3">
         <v>11.618405900166101</v>
       </c>
-      <c r="H22" t="s">
-        <v>56</v>
-      </c>
-      <c r="I22">
-        <v>0.73916245953752302</v>
-      </c>
       <c r="J22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23">
         <v>1.347</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E23">
         <v>0.67247414000000005</v>
       </c>
       <c r="F23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G23">
+        <v>3049.33241</v>
+      </c>
+      <c r="H23" t="s">
+        <v>55</v>
+      </c>
+      <c r="I23" s="3">
         <v>11.334552396527201</v>
       </c>
-      <c r="H23" t="s">
-        <v>56</v>
-      </c>
-      <c r="I23">
-        <v>0.40319962604697202</v>
-      </c>
       <c r="J23" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24">
         <v>1.41</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E24">
         <v>3.1915399999999998</v>
       </c>
       <c r="F24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G24">
+        <v>1977.8261460000001</v>
+      </c>
+      <c r="H24" t="s">
+        <v>55</v>
+      </c>
+      <c r="I24" s="3">
         <v>10.779433804128001</v>
       </c>
-      <c r="H24" t="s">
-        <v>56</v>
-      </c>
-      <c r="I24">
-        <v>0.27510327682400798</v>
-      </c>
       <c r="J24" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25">
         <v>1.35</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E25">
         <v>4.7361000000000004</v>
       </c>
       <c r="F25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G25">
+        <v>1646.5553299999999</v>
+      </c>
+      <c r="H25" t="s">
+        <v>55</v>
+      </c>
+      <c r="I25" s="3">
         <v>10.772894234067399</v>
       </c>
-      <c r="H25" t="s">
-        <v>56</v>
-      </c>
-      <c r="I25">
-        <v>18.263121487151601</v>
-      </c>
       <c r="J25" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26">
         <v>1.6990000000000001</v>
       </c>
       <c r="D26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E26">
         <v>2.9895931999999998</v>
       </c>
       <c r="F26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G26">
+        <v>1761.9487810000001</v>
+      </c>
+      <c r="H26" t="s">
+        <v>55</v>
+      </c>
+      <c r="I26" s="3">
         <v>9.6776504081827497</v>
       </c>
-      <c r="H26" t="s">
-        <v>56</v>
-      </c>
-      <c r="I26">
-        <v>4.3114478153202098</v>
-      </c>
       <c r="J26" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C27">
         <v>1.36</v>
       </c>
       <c r="D27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E27">
         <v>2.13775</v>
       </c>
       <c r="F27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G27">
+        <v>1853.1195339999999</v>
+      </c>
+      <c r="H27" t="s">
+        <v>55</v>
+      </c>
+      <c r="I27" s="3">
         <v>9.6467540399956402</v>
       </c>
-      <c r="H27" t="s">
-        <v>56</v>
-      </c>
-      <c r="I27">
-        <v>3.3393762977146499</v>
-      </c>
       <c r="J27" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28">
         <v>1.323</v>
       </c>
       <c r="D28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E28">
         <v>2.2552509999999999</v>
       </c>
       <c r="F28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G28">
+        <v>1514.89041</v>
+      </c>
+      <c r="H28" t="s">
+        <v>55</v>
+      </c>
+      <c r="I28" s="3">
         <v>9.6237088449384807</v>
       </c>
-      <c r="H28" t="s">
-        <v>56</v>
-      </c>
-      <c r="I28">
-        <v>3.7530796718699202</v>
-      </c>
       <c r="J28" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C29">
         <v>1.7430000000000001</v>
       </c>
       <c r="D29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E29">
         <v>1.7100565999999999</v>
       </c>
       <c r="F29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G29">
+        <v>1896.4139319999999</v>
+      </c>
+      <c r="H29" t="s">
+        <v>55</v>
+      </c>
+      <c r="I29" s="3">
         <v>9.4351414024467299</v>
       </c>
-      <c r="H29" t="s">
-        <v>56</v>
-      </c>
-      <c r="I29">
-        <v>2.5373515206148198</v>
-      </c>
       <c r="J29" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30">
         <v>1.62</v>
       </c>
       <c r="D30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E30">
         <v>2.7057899999999999</v>
       </c>
       <c r="F30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G30">
+        <v>2104.0954080000001</v>
+      </c>
+      <c r="H30" t="s">
+        <v>55</v>
+      </c>
+      <c r="I30" s="3">
         <v>9.4191823909427903</v>
       </c>
-      <c r="H30" t="s">
-        <v>56</v>
-      </c>
-      <c r="I30">
-        <v>2.57755435173017</v>
-      </c>
       <c r="J30" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C31">
         <v>1.528</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31">
         <v>0.92554199999999998</v>
       </c>
       <c r="F31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G31">
+        <v>2425.9743109999999</v>
+      </c>
+      <c r="H31" t="s">
+        <v>55</v>
+      </c>
+      <c r="I31" s="3">
         <v>9.3294952130535993</v>
       </c>
-      <c r="H31" t="s">
-        <v>56</v>
-      </c>
-      <c r="I31">
-        <v>1.5065562427338901</v>
-      </c>
       <c r="J31" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32">
         <v>1.62</v>
       </c>
       <c r="D32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E32">
         <v>3.2440600000000002</v>
       </c>
       <c r="F32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G32">
+        <v>1621.4052690000001</v>
+      </c>
+      <c r="H32" t="s">
+        <v>55</v>
+      </c>
+      <c r="I32" s="3">
         <v>9.2528869281064701</v>
       </c>
-      <c r="H32" t="s">
-        <v>56</v>
-      </c>
-      <c r="I32">
-        <v>4.21307253127652</v>
-      </c>
       <c r="J32" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C33">
         <v>1.38</v>
       </c>
       <c r="D33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E33">
         <v>2.2437499999999999</v>
       </c>
       <c r="F33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G33">
+        <v>1799.902126</v>
+      </c>
+      <c r="H33" t="s">
+        <v>55</v>
+      </c>
+      <c r="I33" s="3">
         <v>9.0529813835346005</v>
       </c>
-      <c r="H33" t="s">
-        <v>56</v>
-      </c>
-      <c r="I33">
-        <v>0.42015228596259602</v>
-      </c>
       <c r="J33" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C34">
         <v>1.415</v>
       </c>
       <c r="D34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E34">
         <v>0.78883851999999999</v>
       </c>
       <c r="F34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G34">
+        <v>2046.3765519999999</v>
+      </c>
+      <c r="H34" t="s">
+        <v>55</v>
+      </c>
+      <c r="I34" s="3">
         <v>9.0386213061430301</v>
       </c>
-      <c r="H34" t="s">
-        <v>56</v>
-      </c>
-      <c r="I34">
-        <v>1.8683192910226101</v>
-      </c>
       <c r="J34" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C35">
         <v>1.91</v>
       </c>
       <c r="D35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E35">
         <v>4.6117093000000002</v>
       </c>
       <c r="F35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G35">
+        <v>1874.7185999999999</v>
+      </c>
+      <c r="H35" t="s">
+        <v>55</v>
+      </c>
+      <c r="I35" s="3">
         <v>8.9483693018497998</v>
       </c>
-      <c r="H35" t="s">
-        <v>56</v>
-      </c>
-      <c r="I35">
-        <v>1.1662380647145301</v>
-      </c>
       <c r="J35" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C36">
         <v>1.5249999999999999</v>
       </c>
       <c r="D36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E36">
         <v>3.0801715999999999</v>
       </c>
       <c r="F36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G36">
+        <v>2019.861101</v>
+      </c>
+      <c r="H36" t="s">
+        <v>55</v>
+      </c>
+      <c r="I36" s="3">
         <v>8.8933900575551892</v>
       </c>
-      <c r="H36" t="s">
-        <v>56</v>
-      </c>
-      <c r="I36">
-        <v>2.5869852782649101</v>
-      </c>
       <c r="J36" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C37">
         <v>1.35</v>
       </c>
       <c r="D37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E37">
         <v>4.1137899999999998</v>
       </c>
       <c r="F37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G37">
+        <v>1701.4979089999999</v>
+      </c>
+      <c r="H37" t="s">
+        <v>55</v>
+      </c>
+      <c r="I37" s="3">
         <v>8.6680402375147807</v>
       </c>
-      <c r="H37" t="s">
-        <v>56</v>
-      </c>
-      <c r="I37">
-        <v>1.95442799585654</v>
-      </c>
       <c r="J37" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C38">
         <v>2.085</v>
       </c>
       <c r="D38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E38">
         <v>4.8101025000000002</v>
       </c>
       <c r="F38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G38">
+        <v>1860.0332020000001</v>
+      </c>
+      <c r="H38" t="s">
+        <v>55</v>
+      </c>
+      <c r="I38" s="3">
         <v>8.6381770770767901</v>
       </c>
-      <c r="H38" t="s">
-        <v>56</v>
-      </c>
-      <c r="I38">
-        <v>12.1207421687738</v>
-      </c>
       <c r="J38" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C39">
         <v>2.0499999999999998</v>
       </c>
       <c r="D39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E39">
         <v>2.6940499999999998</v>
       </c>
       <c r="F39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G39">
+        <v>1873.8076209999999</v>
+      </c>
+      <c r="H39" t="s">
+        <v>55</v>
+      </c>
+      <c r="I39" s="3">
         <v>8.55526962256668</v>
       </c>
-      <c r="H39" t="s">
-        <v>56</v>
-      </c>
-      <c r="I39">
-        <v>4.9496999829715298</v>
-      </c>
       <c r="J39" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C40">
         <v>1.272</v>
       </c>
       <c r="D40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E40">
         <v>5.5514926000000004</v>
       </c>
       <c r="F40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G40">
+        <v>1413.610529</v>
+      </c>
+      <c r="H40" t="s">
+        <v>55</v>
+      </c>
+      <c r="I40" s="3">
         <v>8.3964856120558693</v>
       </c>
-      <c r="H40" t="s">
-        <v>56</v>
-      </c>
-      <c r="I40">
-        <v>0.79894897968737999</v>
-      </c>
       <c r="J40" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C41">
         <v>1.81</v>
       </c>
       <c r="D41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E41">
         <v>3.3448285000000002</v>
       </c>
       <c r="F41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G41">
+        <v>2388.0138000000002</v>
+      </c>
+      <c r="H41" t="s">
+        <v>55</v>
+      </c>
+      <c r="I41" s="3">
         <v>8.1667822738255609</v>
       </c>
-      <c r="H41" t="s">
-        <v>56</v>
-      </c>
-      <c r="I41">
-        <v>2.84758318509301</v>
-      </c>
       <c r="J41" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C42">
         <v>1.67</v>
       </c>
       <c r="D42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E42">
         <v>3.6623800000000002</v>
       </c>
       <c r="F42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G42">
+        <v>1700.784189</v>
+      </c>
+      <c r="H42" t="s">
+        <v>55</v>
+      </c>
+      <c r="I42" s="3">
         <v>7.7875574315332701</v>
       </c>
-      <c r="H42" t="s">
-        <v>56</v>
-      </c>
-      <c r="I42">
-        <v>4.1611278035499604</v>
-      </c>
       <c r="J42" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C43">
         <v>1.44</v>
       </c>
       <c r="D43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E43">
         <v>2.2359835000000001</v>
       </c>
       <c r="F43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G43">
+        <v>1272.7345809999999</v>
+      </c>
+      <c r="H43" t="s">
+        <v>55</v>
+      </c>
+      <c r="I43" s="3">
         <v>7.68090280764536</v>
       </c>
-      <c r="H43" t="s">
-        <v>56</v>
-      </c>
-      <c r="I43">
-        <v>1.4284507622582201</v>
-      </c>
       <c r="J43" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C44">
         <v>1.466</v>
       </c>
       <c r="D44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E44">
         <v>1.7429935000000001</v>
       </c>
       <c r="F44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G44">
+        <v>1496.310943</v>
+      </c>
+      <c r="H44" t="s">
+        <v>55</v>
+      </c>
+      <c r="I44" s="3">
         <v>7.5862748630019103</v>
       </c>
-      <c r="H44" t="s">
-        <v>56</v>
-      </c>
-      <c r="I44">
-        <v>0.88849822559066005</v>
-      </c>
       <c r="J44" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C45">
         <v>1.42</v>
       </c>
       <c r="D45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E45">
         <v>1.84683</v>
       </c>
       <c r="F45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G45">
+        <v>1925.2575469999999</v>
+      </c>
+      <c r="H45" t="s">
+        <v>55</v>
+      </c>
+      <c r="I45" s="3">
         <v>7.5606440943023898</v>
       </c>
-      <c r="H45" t="s">
-        <v>56</v>
-      </c>
-      <c r="I45">
-        <v>1.2391638902773701</v>
-      </c>
       <c r="J45" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46">
         <v>1.56</v>
       </c>
       <c r="D46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E46">
         <v>2.7033900000000002</v>
       </c>
       <c r="F46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G46">
+        <v>1757.9944889999999</v>
+      </c>
+      <c r="H46" t="s">
+        <v>55</v>
+      </c>
+      <c r="I46" s="3">
         <v>7.4937598579876497</v>
       </c>
-      <c r="H46" t="s">
-        <v>56</v>
-      </c>
-      <c r="I46">
-        <v>1.9161205263193499</v>
-      </c>
       <c r="J46" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C47">
         <v>1.58</v>
       </c>
       <c r="D47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E47">
         <v>3.6936399999999998</v>
       </c>
       <c r="F47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G47">
+        <v>1722.7401620000001</v>
+      </c>
+      <c r="H47" t="s">
+        <v>55</v>
+      </c>
+      <c r="I47" s="3">
         <v>7.4170412306108497</v>
       </c>
-      <c r="H47" t="s">
-        <v>56</v>
-      </c>
-      <c r="I47">
-        <v>4.6155871913957496</v>
-      </c>
       <c r="J47" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C48">
         <v>1.385</v>
       </c>
       <c r="D48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E48">
         <v>1.682795</v>
       </c>
       <c r="F48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G48">
+        <v>2238.5596009999999</v>
+      </c>
+      <c r="H48" t="s">
+        <v>55</v>
+      </c>
+      <c r="I48" s="3">
         <v>7.3225226508253201</v>
       </c>
-      <c r="H48" t="s">
-        <v>56</v>
-      </c>
-      <c r="I48">
-        <v>0.84645396356601799</v>
-      </c>
       <c r="J48" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49">
         <v>1.23</v>
       </c>
       <c r="D49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E49">
         <v>2.1846700000000001</v>
       </c>
       <c r="F49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G49">
+        <v>1559.3949009999999</v>
+      </c>
+      <c r="H49" t="s">
+        <v>55</v>
+      </c>
+      <c r="I49" s="3">
         <v>7.2789887697656503</v>
       </c>
-      <c r="H49" t="s">
-        <v>56</v>
-      </c>
-      <c r="I49">
-        <v>1.9358413388170601</v>
-      </c>
       <c r="J49" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C50">
         <v>1.57</v>
       </c>
       <c r="D50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E50">
         <v>2.8717518000000002</v>
       </c>
       <c r="F50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G50">
+        <v>2015.929666</v>
+      </c>
+      <c r="H50" t="s">
+        <v>55</v>
+      </c>
+      <c r="I50" s="3">
         <v>7.1455382143532002</v>
       </c>
-      <c r="H50" t="s">
-        <v>56</v>
-      </c>
-      <c r="I50">
-        <v>2.06188382135098</v>
-      </c>
       <c r="J50" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C51">
         <v>1.74</v>
       </c>
       <c r="D51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E51">
         <v>2.4653</v>
       </c>
       <c r="F51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G51">
+        <v>1792.567196</v>
+      </c>
+      <c r="H51" t="s">
+        <v>55</v>
+      </c>
+      <c r="I51" s="3">
         <v>7.1150016044141102</v>
       </c>
-      <c r="H51" t="s">
-        <v>56</v>
-      </c>
-      <c r="I51">
-        <v>2.0809632778679998</v>
-      </c>
       <c r="J51" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="1" customFormat="1">
       <c r="A52" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C52" s="1">
         <v>0.93</v>
       </c>
       <c r="D52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E52" s="1">
         <v>0.81347499999999995</v>
       </c>
       <c r="F52" t="s">
-        <v>56</v>
-      </c>
-      <c r="G52" s="1">
+        <v>55</v>
+      </c>
+      <c r="G52">
+        <v>1332.5944179999999</v>
+      </c>
+      <c r="H52" t="s">
+        <v>55</v>
+      </c>
+      <c r="I52" s="4">
         <v>7.0369885765334601</v>
       </c>
-      <c r="H52" t="s">
-        <v>56</v>
-      </c>
-      <c r="I52" s="1">
-        <v>0.72355573774410398</v>
-      </c>
       <c r="J52" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>